<commit_message>
feat: build go with os windows output main.exe
</commit_message>
<xml_diff>
--- a/files/angsuran.xlsx
+++ b/files/angsuran.xlsx
@@ -44,31 +44,31 @@
     <t>2019-01-10</t>
   </si>
   <si>
+    <t>2019-06-10</t>
+  </si>
+  <si>
+    <t>2019-05-10</t>
+  </si>
+  <si>
+    <t>2018-09-10</t>
+  </si>
+  <si>
+    <t>2019-03-10</t>
+  </si>
+  <si>
     <t>2019-02-10</t>
   </si>
   <si>
-    <t>2019-03-10</t>
+    <t>2018-11-10</t>
+  </si>
+  <si>
+    <t>2018-10-10</t>
+  </si>
+  <si>
+    <t>2018-08-10</t>
   </si>
   <si>
     <t>2019-04-10</t>
-  </si>
-  <si>
-    <t>2019-05-10</t>
-  </si>
-  <si>
-    <t>2019-06-10</t>
-  </si>
-  <si>
-    <t>2018-08-10</t>
-  </si>
-  <si>
-    <t>2018-11-10</t>
-  </si>
-  <si>
-    <t>2018-09-10</t>
-  </si>
-  <si>
-    <t>2018-10-10</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>856074.82</v>
@@ -433,7 +433,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>856074.82</v>
@@ -453,7 +453,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>856074.82</v>
@@ -473,7 +473,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>856074.82</v>
@@ -533,7 +533,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>856074.82</v>
@@ -553,7 +553,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <v>856074.82</v>
@@ -573,7 +573,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C10">
         <v>856074.82</v>
@@ -593,7 +593,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>856074.82</v>
@@ -613,7 +613,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <v>856074.82</v>

</xml_diff>

<commit_message>
feat: add volumes docker mapping for xlsx file
</commit_message>
<xml_diff>
--- a/files/angsuran.xlsx
+++ b/files/angsuran.xlsx
@@ -35,40 +35,40 @@
     <t>Sisa Pinjaman</t>
   </si>
   <si>
+    <t>2019-01-10</t>
+  </si>
+  <si>
     <t>2019-07-10</t>
   </si>
   <si>
+    <t>2018-11-10</t>
+  </si>
+  <si>
+    <t>2019-05-10</t>
+  </si>
+  <si>
+    <t>2019-02-10</t>
+  </si>
+  <si>
+    <t>2018-09-10</t>
+  </si>
+  <si>
+    <t>2019-06-10</t>
+  </si>
+  <si>
+    <t>2018-10-10</t>
+  </si>
+  <si>
+    <t>2019-03-10</t>
+  </si>
+  <si>
     <t>2018-12-10</t>
   </si>
   <si>
-    <t>2019-01-10</t>
-  </si>
-  <si>
-    <t>2019-06-10</t>
-  </si>
-  <si>
-    <t>2019-05-10</t>
-  </si>
-  <si>
-    <t>2018-09-10</t>
-  </si>
-  <si>
-    <t>2019-03-10</t>
-  </si>
-  <si>
-    <t>2019-02-10</t>
-  </si>
-  <si>
-    <t>2018-11-10</t>
-  </si>
-  <si>
-    <t>2018-10-10</t>
+    <t>2019-04-10</t>
   </si>
   <si>
     <t>2018-08-10</t>
-  </si>
-  <si>
-    <t>2019-04-10</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>856074.82</v>
@@ -453,7 +453,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>856074.82</v>
@@ -473,7 +473,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>856074.82</v>
@@ -493,7 +493,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>856074.82</v>
@@ -513,7 +513,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>856074.82</v>
@@ -533,7 +533,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>856074.82</v>
@@ -553,7 +553,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>856074.82</v>
@@ -573,7 +573,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10">
         <v>856074.82</v>
@@ -593,7 +593,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>856074.82</v>
@@ -613,7 +613,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <v>856074.82</v>
@@ -633,7 +633,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13">
         <v>856074.82</v>

</xml_diff>